<commit_message>
Corrected test cases for .Drop
</commit_message>
<xml_diff>
--- a/Examples/images/test cases.xlsx
+++ b/Examples/images/test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="280" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RPN Calculator" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>.Push</t>
   </si>
@@ -60,9 +60,6 @@
     <t>[], 0</t>
   </si>
   <si>
-    <t>[1], 2</t>
-  </si>
-  <si>
     <t>.Calculate</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>[], 1</t>
   </si>
 </sst>
 </file>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -535,13 +535,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -590,13 +590,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -615,106 +615,94 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
         <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>